<commit_message>
updated spreadsheets > title
</commit_message>
<xml_diff>
--- a/public/spreadsheets/townportal-computers.xlsx
+++ b/public/spreadsheets/townportal-computers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Desktop\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\townportal-capstone-2-lv8\public\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4652CA03-1B6A-498B-A828-588CE898CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9EF9B-9E6C-472B-8EB7-4DA640927AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>COMPUTERS</t>
+    <t>LIST OF COMPUTERS</t>
   </si>
 </sst>
 </file>
@@ -653,17 +653,17 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="9" customWidth="1"/>
-    <col min="2" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="9" customWidth="1"/>
+    <col min="2" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -672,35 +672,35 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
@@ -709,21 +709,21 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="4"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
@@ -743,30 +743,30 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="13" spans="1:8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
     </row>
-    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
     </row>
-    <row r="16" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
     </row>
   </sheetData>

</xml_diff>